<commit_message>
new design for question decided, saving progress before change
</commit_message>
<xml_diff>
--- a/utils/Notes/Formula.xlsx
+++ b/utils/Notes/Formula.xlsx
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:K45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,7 +615,7 @@
       </c>
       <c r="B4" s="2">
         <f>O5</f>
-        <v>-1</v>
+        <v>-0.2</v>
       </c>
       <c r="C4" t="s">
         <v>15</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="3">
         <v>1</v>
@@ -684,18 +684,18 @@
       </c>
       <c r="L5">
         <f>B5</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
         <f>MAX(0,O7)/K7+MAX(0,O8)/K8</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5:O8" si="0">ROUND((L5+M5-N5)/SUM(L5:N5,0.0000000001),2)</f>
-        <v>-1</v>
+        <v>-0.2</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.2">
@@ -729,7 +729,7 @@
       </c>
       <c r="B7" s="2">
         <f>O8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>6</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>7</v>
@@ -770,7 +770,7 @@
       </c>
       <c r="L8">
         <f>B8</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -780,7 +780,7 @@
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.2">
@@ -1316,11 +1316,11 @@
     <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="C29" s="2">
         <f>O30</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2">
         <f>O31</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29" t="s">
         <v>6</v>
@@ -1366,24 +1366,24 @@
       </c>
       <c r="M30">
         <f>MAX(0,O32)/K32+MAX(0,O33)/K33</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="N30">
         <v>0</v>
       </c>
       <c r="O30">
         <f>ROUND((L30+M30-N30)/SUM(L30:N30,0.0000000001),2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <f>O32</f>
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
       <c r="D31" s="2">
         <f>O33</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F31" s="2">
         <f>O34</f>
@@ -1408,19 +1408,19 @@
       </c>
       <c r="N31">
         <f>MAX(0,O33)/K33</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O31">
         <f>ROUND((L31+M31-N31)/SUM(L31:N31,0.0000000001),2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -1436,18 +1436,18 @@
       </c>
       <c r="L32">
         <f>B32</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32">
         <f>MAX(0,O34)/K34+MAX(0,O35)/K35</f>
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="O32">
         <f t="shared" ref="O32:O35" si="3">ROUND((L32+M32-N32)/SUM(L32:N32,0.0000000001),2)</f>
-        <v>-0.2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
@@ -1462,7 +1462,7 @@
       </c>
       <c r="L33">
         <f>D32</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M33">
         <v>0</v>
@@ -1472,13 +1472,13 @@
       </c>
       <c r="O33">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
         <f>O35</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>6</v>
@@ -1506,7 +1506,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B35" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35">
         <v>7</v>
@@ -1519,7 +1519,7 @@
       </c>
       <c r="L35">
         <f>B35</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M35">
         <v>0</v>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="O35">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
@@ -1554,22 +1554,22 @@
     <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G39" s="5">
         <f>G40/(G40+I40)</f>
-        <v>0.8571428571428571</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="5">
         <f>I40/(G40+I40)</f>
-        <v>0.14285714285714285</v>
+        <v>0.42857142857142855</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G40" s="7">
         <f>(C29+C20+C11+C2)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I40" s="7">
         <f>(E29+E20+E11+E2)</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.2">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="H41" s="8">
         <f>D31+D22+D13+D4</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J41" s="8">
         <f>F31+F22+F13+F4</f>

</xml_diff>